<commit_message>
Added function to print test statuses and severity summary to the console
</commit_message>
<xml_diff>
--- a/templates/test-results-template.xlsx
+++ b/templates/test-results-template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20357"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\cdmgtri\niem-test-suite\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\model\niem-model-qa\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6455EC-D0FE-4865-AE03-39FF318C8362}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="936" yWindow="0" windowWidth="23076" windowHeight="10320"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="23070" windowHeight="10320" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="6" r:id="rId1"/>
@@ -144,7 +145,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -807,54 +808,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="36.109375" style="11" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="36.140625" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="13"/>
     </row>
-    <row r="3" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="20"/>
     </row>
-    <row r="4" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="15"/>
     </row>
-    <row r="5" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="15"/>
     </row>
-    <row r="6" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>27</v>
       </c>
       <c r="B6" s="14"/>
     </row>
-    <row r="7" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>28</v>
       </c>
       <c r="B7" s="14"/>
     </row>
-    <row r="8" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>29</v>
       </c>
@@ -890,7 +891,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -898,12 +899,12 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="11.77734375" customWidth="1"/>
+    <col min="1" max="5" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>18</v>
       </c>
@@ -921,7 +922,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1"/>
+  <autoFilter ref="A1:E1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <conditionalFormatting sqref="A2:A1048576">
     <cfRule type="expression" dxfId="17" priority="13" stopIfTrue="1">
       <formula>AND($C2=0, $D2=0, $E2=0, $A2&lt;&gt;"")</formula>
@@ -946,7 +947,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -954,22 +955,22 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="40.44140625" style="3" customWidth="1"/>
-    <col min="4" max="5" width="8.88671875" style="3"/>
-    <col min="6" max="6" width="17.88671875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="3"/>
-    <col min="8" max="8" width="12.77734375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="5.88671875" style="9" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="40.42578125" style="3" customWidth="1"/>
+    <col min="4" max="5" width="8.85546875" style="3"/>
+    <col min="6" max="6" width="17.85546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="3"/>
+    <col min="8" max="8" width="12.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="5.85546875" style="9" customWidth="1"/>
     <col min="10" max="10" width="8" style="18" customWidth="1"/>
-    <col min="11" max="12" width="28.77734375" style="3" customWidth="1"/>
-    <col min="13" max="16" width="17.109375" style="3" customWidth="1"/>
+    <col min="11" max="12" width="28.7109375" style="3" customWidth="1"/>
+    <col min="13" max="16" width="17.140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1020,7 +1021,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P1"/>
+  <autoFilter ref="A1:P1" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="expression" dxfId="12" priority="2">
       <formula>AND($D1="fail", $B1="info")</formula>
@@ -1049,7 +1050,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1057,21 +1058,21 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="40.44140625" style="3" customWidth="1"/>
-    <col min="4" max="5" width="8.88671875" style="3"/>
-    <col min="6" max="6" width="17.88671875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="3"/>
-    <col min="8" max="8" width="12.77734375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="5.88671875" style="9" customWidth="1"/>
-    <col min="10" max="11" width="28.77734375" style="3" customWidth="1"/>
-    <col min="12" max="15" width="17.109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="40.42578125" style="3" customWidth="1"/>
+    <col min="4" max="5" width="8.85546875" style="3"/>
+    <col min="6" max="6" width="17.85546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="3"/>
+    <col min="8" max="8" width="12.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="5.85546875" style="9" customWidth="1"/>
+    <col min="10" max="11" width="28.7109375" style="3" customWidth="1"/>
+    <col min="12" max="15" width="17.140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1118,104 +1119,104 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I2" s="16"/>
       <c r="J2" s="17"/>
       <c r="K2" s="17"/>
       <c r="L2" s="17"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I3" s="16"/>
       <c r="J3" s="17"/>
       <c r="K3" s="17"/>
       <c r="L3" s="17"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I4" s="16"/>
       <c r="J4" s="17"/>
       <c r="K4" s="17"/>
       <c r="L4" s="17"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I5" s="16"/>
       <c r="J5" s="17"/>
       <c r="K5" s="17"/>
       <c r="L5" s="17"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I6" s="16"/>
       <c r="J6" s="17"/>
       <c r="K6" s="17"/>
       <c r="L6" s="17"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I7" s="16"/>
       <c r="J7" s="17"/>
       <c r="K7" s="17"/>
       <c r="L7" s="17"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I8" s="16"/>
       <c r="J8" s="17"/>
       <c r="K8" s="17"/>
       <c r="L8" s="17"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I9" s="16"/>
       <c r="J9" s="17"/>
       <c r="K9" s="17"/>
       <c r="L9" s="17"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I10" s="16"/>
       <c r="J10" s="17"/>
       <c r="K10" s="17"/>
       <c r="L10" s="17"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I11" s="16"/>
       <c r="J11" s="17"/>
       <c r="K11" s="17"/>
       <c r="L11" s="17"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I12" s="16"/>
       <c r="J12" s="17"/>
       <c r="K12" s="17"/>
       <c r="L12" s="17"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I13" s="16"/>
       <c r="J13" s="17"/>
       <c r="K13" s="17"/>
       <c r="L13" s="17"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I14" s="16"/>
       <c r="J14" s="17"/>
       <c r="K14" s="17"/>
       <c r="L14" s="17"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I15" s="16"/>
       <c r="J15" s="17"/>
       <c r="K15" s="17"/>
       <c r="L15" s="17"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I16" s="16"/>
       <c r="J16" s="17"/>
       <c r="K16" s="17"/>
       <c r="L16" s="17"/>
     </row>
-    <row r="17" spans="9:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I17" s="16"/>
       <c r="J17" s="17"/>
       <c r="K17" s="17"/>
       <c r="L17" s="17"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O1"/>
+  <autoFilter ref="A1:O1" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="expression" dxfId="6" priority="3">
       <formula>$B1="info"</formula>
@@ -1238,29 +1239,29 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="40.44140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="23.44140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="18.77734375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="30.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="40.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="3"/>
     <col min="9" max="9" width="10" style="3" customWidth="1"/>
-    <col min="10" max="10" width="38.109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="38.140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1292,7 +1293,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -1305,7 +1306,7 @@
       <c r="J2" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J2"/>
+  <autoFilter ref="A1:J2" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="expression" dxfId="2" priority="6">
       <formula>$B1="warning"</formula>

</xml_diff>